<commit_message>
ExcelHelper: read Image column ImageConverter:  check null
</commit_message>
<xml_diff>
--- a/Shoping/Book1.xlsx
+++ b/Shoping/Book1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9192" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Paid</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Vouchers</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>C:\Users\admin\Desktop\bmw.jpg</t>
   </si>
 </sst>
 </file>
@@ -363,34 +369,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>40</v>
       </c>
       <c r="B2">
         <v>123</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>456</v>
       </c>
@@ -398,7 +411,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>123</v>
       </c>
@@ -412,13 +425,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>